<commit_message>
Updates to COTS and Prelim Spec
Updated formatting on COTS analysis. Added power requirements to
Prelim_Spec.
</commit_message>
<xml_diff>
--- a/Misc/Design Documents/COTS Analysis.xlsx
+++ b/Misc/Design Documents/COTS Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="80">
   <si>
     <t>Criteria</t>
   </si>
@@ -241,6 +241,30 @@
   </si>
   <si>
     <t>$59.99($0 from dave)</t>
+  </si>
+  <si>
+    <t>Weightings</t>
+  </si>
+  <si>
+    <t>Cost Ratings</t>
+  </si>
+  <si>
+    <t>Processor Ratings</t>
+  </si>
+  <si>
+    <t>Memory Ratings</t>
+  </si>
+  <si>
+    <t>USB Ratings</t>
+  </si>
+  <si>
+    <t>Power Ratings</t>
+  </si>
+  <si>
+    <t>HDMI Ratings</t>
+  </si>
+  <si>
+    <t>Final Scores</t>
   </si>
 </sst>
 </file>
@@ -250,10 +274,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -343,11 +373,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -377,12 +442,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -679,10 +760,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -928,7 +1009,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -937,10 +1018,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,747 +1041,737 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>50</v>
+      <c r="A1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="22"/>
+      <c r="S1" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D3" s="5">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E3" s="5">
         <v>9</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F3" s="5">
         <v>7</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G3" s="5">
         <v>9</v>
       </c>
-      <c r="H2" s="2">
-        <f>AVERAGE(B2:G2)</f>
+      <c r="H3" s="2">
+        <f>AVERAGE(B3:G3)</f>
         <v>7.333333333333333</v>
       </c>
-      <c r="I2" s="2">
-        <f>H2/SUM($H$2:$H$7)</f>
+      <c r="I3" s="2">
+        <f>H3/SUM($H$3:$H$8)</f>
         <v>0.42395693135935403</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="10">
-        <v>1</v>
-      </c>
-      <c r="M2" s="10">
-        <v>1</v>
-      </c>
-      <c r="N2" s="10">
-        <v>1</v>
-      </c>
-      <c r="O2" s="10">
-        <v>1</v>
-      </c>
-      <c r="P2" s="10">
-        <f>AVERAGE(L2:O2)</f>
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2">
-        <f>P2/$P$6</f>
+      <c r="L3" s="10">
+        <v>1</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1</v>
+      </c>
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10">
+        <v>1</v>
+      </c>
+      <c r="P3" s="10">
+        <f>AVERAGE(L3:O3)</f>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>P3/$P$7</f>
         <v>0.25</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
-        <f>I2</f>
+      <c r="S3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2">
+        <f>I3</f>
         <v>0.42395693135935403</v>
       </c>
-      <c r="U2" s="2">
-        <f>Q2</f>
-        <v>0.25</v>
-      </c>
-      <c r="V2" s="2">
+      <c r="U3" s="2">
         <f>Q3</f>
         <v>0.25</v>
       </c>
-      <c r="W2" s="2">
+      <c r="V3" s="2">
         <f>Q4</f>
         <v>0.25</v>
       </c>
-      <c r="X2" s="2">
+      <c r="W3" s="2">
         <f>Q5</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>3</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7</v>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H7" si="0">AVERAGE(B3:G3)</f>
-        <v>3.5185185185185186</v>
-      </c>
-      <c r="I3" s="2">
-        <f t="shared" ref="I3:I7" si="1">H3/SUM($H$2:$H$7)</f>
-        <v>0.20341367918756886</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="10">
-        <v>1</v>
-      </c>
-      <c r="M3" s="10">
-        <v>1</v>
-      </c>
-      <c r="N3" s="10">
-        <v>1</v>
-      </c>
-      <c r="O3" s="10">
-        <v>1</v>
-      </c>
-      <c r="P3" s="10">
-        <f t="shared" ref="P3:P5" si="2">AVERAGE(L3:O3)</f>
-        <v>1</v>
-      </c>
-      <c r="Q3" s="2">
-        <f t="shared" ref="Q3:Q5" si="3">P3/$P$6</f>
+      <c r="X3" s="2">
+        <f>Q6</f>
         <v>0.25</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="2">
-        <f t="shared" ref="T3:T7" si="4">I3</f>
-        <v>0.20341367918756886</v>
-      </c>
-      <c r="U3" s="2">
-        <f>Q10</f>
-        <v>0.51166568222090958</v>
-      </c>
-      <c r="V3" s="2">
-        <f>Q11</f>
-        <v>0.30699940933254571</v>
-      </c>
-      <c r="W3" s="2">
-        <f>Q12</f>
-        <v>3.5144713526284697E-2</v>
-      </c>
-      <c r="X3" s="2">
-        <f>Q13</f>
-        <v>0.14619019492025989</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C4" s="6">
-        <v>0.2</v>
+      <c r="C4" s="5">
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="6">
-        <v>0.33333333333333331</v>
+      <c r="F4" s="5">
+        <v>3</v>
       </c>
       <c r="G4" s="5">
         <v>7</v>
       </c>
       <c r="H4" s="2">
+        <f t="shared" ref="H4:H8" si="0">AVERAGE(B4:G4)</f>
+        <v>3.5185185185185186</v>
+      </c>
+      <c r="I4" s="2">
+        <f>H4/SUM($H$3:$H$8)</f>
+        <v>0.20341367918756886</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="10">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="10">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" ref="P4:P6" si="1">AVERAGE(L4:O4)</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>P4/$P$7</f>
+        <v>0.25</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" ref="T4:T8" si="2">I4</f>
+        <v>0.20341367918756886</v>
+      </c>
+      <c r="U4" s="2">
+        <f>Q11</f>
+        <v>0.51166568222090958</v>
+      </c>
+      <c r="V4" s="2">
+        <f>Q12</f>
+        <v>0.30699940933254571</v>
+      </c>
+      <c r="W4" s="2">
+        <f>Q13</f>
+        <v>3.5144713526284697E-2</v>
+      </c>
+      <c r="X4" s="2">
+        <f>Q14</f>
+        <v>0.14619019492025989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G5" s="5">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="0"/>
         <v>2.2740740740740741</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I5" s="2">
+        <f>H5/SUM($H$3:$H$8)</f>
+        <v>0.1314694726538603</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1</v>
+      </c>
+      <c r="N5" s="10">
+        <v>1</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>P5/$P$7</f>
+        <v>0.25</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" si="2"/>
         <v>0.1314694726538603</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="10">
-        <v>1</v>
-      </c>
-      <c r="M4" s="10">
-        <v>1</v>
-      </c>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="10">
-        <v>1</v>
-      </c>
-      <c r="P4" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T4" s="2">
-        <f t="shared" si="4"/>
-        <v>0.1314694726538603</v>
-      </c>
-      <c r="U4" s="2">
-        <f>Q18</f>
-        <v>0.37499999999999994</v>
-      </c>
-      <c r="V4" s="2">
+      <c r="U5" s="2">
         <f>Q19</f>
         <v>0.37499999999999994</v>
       </c>
-      <c r="W4" s="2">
+      <c r="V5" s="2">
         <f>Q20</f>
-        <v>0.12499999999999999</v>
-      </c>
-      <c r="X4" s="2">
+        <v>0.37499999999999994</v>
+      </c>
+      <c r="W5" s="2">
         <f>Q21</f>
         <v>0.12499999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="X5" s="2">
+        <f>Q22</f>
+        <v>0.12499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="6">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C6" s="6">
         <v>0.2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D6" s="6">
         <v>0.2</v>
       </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
         <v>0.2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G6" s="5">
         <v>3</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
         <v>0.78518518518518521</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I6" s="2">
+        <f>H6/SUM($H$3:$H$8)</f>
+        <v>4.5393368408173262E-2</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="10">
+        <v>1</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10">
+        <v>1</v>
+      </c>
+      <c r="P6" s="10">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>P6/$P$7</f>
+        <v>0.25</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="2"/>
         <v>4.5393368408173262E-2</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1</v>
-      </c>
-      <c r="M5" s="10">
-        <v>1</v>
-      </c>
-      <c r="N5" s="10">
-        <v>1</v>
-      </c>
-      <c r="O5" s="10">
-        <v>1</v>
-      </c>
-      <c r="P5" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="Q5" s="2">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="T5" s="2">
-        <f t="shared" si="4"/>
-        <v>4.5393368408173262E-2</v>
-      </c>
-      <c r="U5" s="2">
-        <f>Q26</f>
-        <v>0.37878787878787878</v>
-      </c>
-      <c r="V5" s="2">
+      <c r="U6" s="2">
         <f>Q27</f>
         <v>0.37878787878787878</v>
       </c>
-      <c r="W5" s="2">
+      <c r="V6" s="2">
         <f>Q28</f>
+        <v>0.37878787878787878</v>
+      </c>
+      <c r="W6" s="2">
+        <f>Q29</f>
         <v>0.17676767676767677</v>
       </c>
-      <c r="X5" s="2">
-        <f>Q29</f>
+      <c r="X6" s="2">
+        <f>Q30</f>
         <v>6.5656565656565663E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="6">
         <v>0.14285714285714285</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E7" s="6">
         <v>5</v>
       </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
         <v>9</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
         <v>3.0793650793650791</v>
       </c>
-      <c r="I6" s="2">
-        <f t="shared" si="1"/>
+      <c r="I7" s="2">
+        <f>H7/SUM($H$3:$H$8)</f>
         <v>0.17802520494310536</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="10">
-        <f>SUM(P2:P5)</f>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="10">
+        <f>SUM(P3:P6)</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="2"/>
-      <c r="S6" s="2" t="s">
+      <c r="Q7" s="2"/>
+      <c r="S7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="2">
-        <f t="shared" si="4"/>
+      <c r="T7" s="2">
+        <f t="shared" si="2"/>
         <v>0.17802520494310536</v>
       </c>
-      <c r="U6" s="2">
-        <f>Q34</f>
+      <c r="U7" s="2">
+        <f>Q35</f>
         <v>6.3844086021505375E-2</v>
       </c>
-      <c r="V6" s="2">
-        <f>Q35</f>
+      <c r="V7" s="2">
+        <f>Q36</f>
         <v>0.18817204301075269</v>
       </c>
-      <c r="W6" s="2">
-        <f>Q36</f>
+      <c r="W7" s="2">
+        <f>Q37</f>
         <v>0.18346774193548387</v>
       </c>
-      <c r="X6" s="2">
-        <f>Q37</f>
+      <c r="X7" s="2">
+        <f>Q38</f>
         <v>0.56451612903225812</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B8" s="7">
         <v>0.1111111111111111</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="7">
         <v>0.14285714285714285</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="7">
         <v>0.14285714285714285</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="7">
         <v>0.1111111111111111</v>
       </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
         <v>0.30687830687830686</v>
       </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
+      <c r="I8" s="2">
+        <f>H8/SUM($H$3:$H$8)</f>
         <v>1.7741343447938335E-2</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="T7" s="2">
-        <f t="shared" si="4"/>
+      <c r="T8" s="2">
+        <f t="shared" si="2"/>
         <v>1.7741343447938335E-2</v>
       </c>
-      <c r="U7" s="2">
-        <f>Q42</f>
-        <v>0.3</v>
-      </c>
-      <c r="V7" s="2">
+      <c r="U8" s="2">
         <f>Q43</f>
         <v>0.3</v>
       </c>
-      <c r="W7" s="2">
+      <c r="V8" s="2">
         <f>Q44</f>
         <v>0.3</v>
       </c>
-      <c r="X7" s="2">
+      <c r="W8" s="2">
         <f>Q45</f>
+        <v>0.3</v>
+      </c>
+      <c r="X8" s="2">
+        <f>Q46</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="S8" s="13" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="K9" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="22"/>
+      <c r="S9" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13">
-        <f>SUM(U2*$T$2+U3*$T$3+U4*$T$4+U5*$T$5+U6*$T$6+U7*$T$7)</f>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13">
+        <f>SUM(U3*$T$3+U4*$T$4+U5*$T$5+U6*$T$6+U7*$T$7+U8*$T$8)</f>
         <v>0.29325280128274261</v>
       </c>
-      <c r="V8" s="13">
-        <f t="shared" ref="V8:X8" si="5">SUM(V2*$T$2+V3*$T$3+V4*$T$4+V5*$T$5+V6*$T$6+V7*$T$7)</f>
+      <c r="V9" s="13">
+        <f>SUM(V3*$T$3+V4*$T$4+V5*$T$5+V6*$T$6+V7*$T$7+V8*$T$8)</f>
         <v>0.27375439173208194</v>
       </c>
-      <c r="W8" s="13">
-        <f t="shared" si="5"/>
+      <c r="W9" s="13">
+        <f>SUM(W3*$T$3+W4*$T$4+W5*$T$5+W6*$T$6+W7*$T$7+W8*$T$8)</f>
         <v>0.17558019807101255</v>
       </c>
-      <c r="X8" s="13">
-        <f t="shared" si="5"/>
+      <c r="X9" s="13">
+        <f>SUM(X3*$T$3+X4*$T$4+X5*$T$5+X6*$T$6+X7*$T$7+X8*$T$8)</f>
         <v>0.25741260891416295</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="10">
-        <v>1</v>
-      </c>
-      <c r="M10" s="10">
-        <v>5</v>
-      </c>
-      <c r="N10" s="10">
-        <v>9</v>
-      </c>
-      <c r="O10" s="10">
-        <v>7</v>
-      </c>
-      <c r="P10" s="10">
-        <f>AVERAGE(L10:O10)</f>
-        <v>5.5</v>
-      </c>
-      <c r="Q10" s="2">
-        <f>P10/$P$14</f>
-        <v>0.51166568222090958</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K11" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L11" s="10">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="M11" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N11" s="10">
+        <v>9</v>
+      </c>
+      <c r="O11" s="10">
         <v>7</v>
       </c>
-      <c r="O11" s="10">
-        <v>5</v>
-      </c>
       <c r="P11" s="10">
-        <f t="shared" ref="P11:P13" si="6">AVERAGE(L11:O11)</f>
-        <v>3.3</v>
+        <f>AVERAGE(L11:O11)</f>
+        <v>5.5</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" ref="Q11:Q13" si="7">P11/$P$14</f>
-        <v>0.30699940933254571</v>
-      </c>
-      <c r="S11" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="T11" s="17"/>
+        <f>P11/$P$15</f>
+        <v>0.51166568222090958</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K12" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L12" s="10">
-        <v>0.1111111111111111</v>
+        <v>0.2</v>
       </c>
       <c r="M12" s="10">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="N12" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O12" s="10">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="P12" s="10">
-        <f t="shared" si="6"/>
-        <v>0.37777777777777777</v>
+        <f t="shared" ref="P12:P14" si="3">AVERAGE(L12:O12)</f>
+        <v>3.3</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" si="7"/>
-        <v>3.5144713526284697E-2</v>
-      </c>
-      <c r="S12" s="17">
-        <f>U8</f>
-        <v>0.29325280128274261</v>
-      </c>
-      <c r="T12" s="17" t="s">
-        <v>49</v>
-      </c>
+        <f>P12/$P$15</f>
+        <v>0.30699940933254571</v>
+      </c>
+      <c r="S12" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="T12" s="25"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="N13" s="10">
+        <v>1</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="P13" s="10">
+        <f t="shared" si="3"/>
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="Q13" s="2">
+        <f>P13/$P$15</f>
+        <v>3.5144713526284697E-2</v>
+      </c>
+      <c r="S13" s="21">
+        <f>U9</f>
+        <v>0.29325280128274261</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L14" s="10">
         <v>0.14285714285714285</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M14" s="10">
         <v>0.14285714285714285</v>
       </c>
-      <c r="N13" s="10">
+      <c r="N14" s="10">
         <v>5</v>
       </c>
-      <c r="O13" s="10">
-        <v>1</v>
-      </c>
-      <c r="P13" s="10">
-        <f t="shared" si="6"/>
+      <c r="O14" s="10">
+        <v>1</v>
+      </c>
+      <c r="P14" s="10">
+        <f t="shared" si="3"/>
         <v>1.5714285714285714</v>
       </c>
-      <c r="Q13" s="2">
-        <f t="shared" si="7"/>
+      <c r="Q14" s="2">
+        <f>P14/$P$15</f>
         <v>0.14619019492025989</v>
       </c>
-      <c r="S13" s="17">
-        <f>V8</f>
+      <c r="S14" s="21">
+        <f>V9</f>
         <v>0.27375439173208194</v>
       </c>
-      <c r="T13" s="17" t="s">
+      <c r="T14" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="10">
-        <f>SUM(P10:P13)</f>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="10">
+        <f>SUM(P11:P14)</f>
         <v>10.74920634920635</v>
       </c>
-      <c r="Q14" s="2"/>
-      <c r="S14" s="17">
-        <f>W8</f>
+      <c r="Q15" s="2"/>
+      <c r="S15" s="21">
+        <f>W9</f>
         <v>0.17558019807101255</v>
       </c>
-      <c r="T14" s="17" t="s">
+      <c r="T15" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="S15" s="17">
-        <f>X8</f>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S16" s="21">
+        <f>X9</f>
         <v>0.25741260891416295</v>
       </c>
-      <c r="T15" s="17" t="s">
+      <c r="T16" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
+      <c r="K17" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" s="22"/>
+    </row>
+    <row r="18" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P17" s="2" t="s">
+      <c r="P18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="Q18" s="2" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L18" s="10">
-        <v>1</v>
-      </c>
-      <c r="M18" s="10">
-        <v>1</v>
-      </c>
-      <c r="N18" s="10">
-        <v>3</v>
-      </c>
-      <c r="O18" s="10">
-        <v>3</v>
-      </c>
-      <c r="P18" s="10">
-        <f>AVERAGE(L18:O18)</f>
-        <v>2</v>
-      </c>
-      <c r="Q18" s="2">
-        <f>P18/$P$22</f>
-        <v>0.37499999999999994</v>
-      </c>
-      <c r="S18" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="T18" s="19" t="str">
-        <f>VLOOKUP(LARGE(S12:S15,1),S12:T15,2,FALSE)</f>
-        <v>Pi 3</v>
       </c>
     </row>
     <row r="19" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K19" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L19" s="10">
         <v>1</v>
@@ -1715,44 +1786,51 @@
         <v>3</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" ref="P19:P21" si="8">AVERAGE(L19:O19)</f>
+        <f>AVERAGE(L19:O19)</f>
         <v>2</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" ref="Q19:Q21" si="9">P19/$P$22</f>
+        <f>P19/$P$23</f>
         <v>0.37499999999999994</v>
       </c>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
+      <c r="S19" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="T19" s="18" t="str">
+        <f>VLOOKUP(LARGE(S13:S16,1),S13:T16,2,FALSE)</f>
+        <v>Pi 3</v>
+      </c>
     </row>
     <row r="20" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L20" s="10">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M20" s="10">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="N20" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O20" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="8"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" ref="P20:P22" si="4">AVERAGE(L20:O20)</f>
+        <v>2</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="9"/>
-        <v>0.12499999999999999</v>
-      </c>
+        <f>P20/$P$23</f>
+        <v>0.37499999999999994</v>
+      </c>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
     </row>
     <row r="21" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K21" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L21" s="10">
         <v>0.33333333333333331</v>
@@ -1767,75 +1845,81 @@
         <v>1</v>
       </c>
       <c r="P21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="9"/>
+        <f>P21/$P$23</f>
         <v>0.12499999999999999</v>
       </c>
     </row>
     <row r="22" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L22" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M22" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N22" s="10">
+        <v>1</v>
+      </c>
+      <c r="O22" s="10">
+        <v>1</v>
+      </c>
       <c r="P22" s="10">
-        <f>SUM(P18:P21)</f>
+        <f t="shared" si="4"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Q22" s="2">
+        <f>P22/$P$23</f>
+        <v>0.12499999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="10">
+        <f>SUM(P19:P22)</f>
         <v>5.3333333333333339</v>
       </c>
-      <c r="Q22" s="2"/>
+      <c r="Q23" s="2"/>
     </row>
     <row r="25" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K25" s="2"/>
-      <c r="L25" s="2" t="s">
+      <c r="K25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" s="22"/>
+    </row>
+    <row r="26" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P25" s="2" t="s">
+      <c r="P26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="Q26" s="2" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L26" s="10">
-        <v>1</v>
-      </c>
-      <c r="M26" s="10">
-        <v>1</v>
-      </c>
-      <c r="N26" s="10">
-        <v>3</v>
-      </c>
-      <c r="O26" s="10">
-        <v>5</v>
-      </c>
-      <c r="P26" s="10">
-        <f>AVERAGE(L26:O26)</f>
-        <v>2.5</v>
-      </c>
-      <c r="Q26" s="2">
-        <f>P26/$P$30</f>
-        <v>0.37878787878787878</v>
       </c>
     </row>
     <row r="27" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L27" s="10">
         <v>1</v>
@@ -1850,150 +1934,156 @@
         <v>5</v>
       </c>
       <c r="P27" s="10">
-        <f t="shared" ref="P27:P29" si="10">AVERAGE(L27:O27)</f>
+        <f>AVERAGE(L27:O27)</f>
         <v>2.5</v>
       </c>
       <c r="Q27" s="2">
-        <f t="shared" ref="Q27:Q29" si="11">P27/$P$30</f>
+        <f>P27/$P$31</f>
         <v>0.37878787878787878</v>
       </c>
     </row>
     <row r="28" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L28" s="10">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M28" s="10">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="N28" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O28" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P28" s="10">
-        <f t="shared" si="10"/>
-        <v>1.1666666666666665</v>
+        <f t="shared" ref="P28:P30" si="5">AVERAGE(L28:O28)</f>
+        <v>2.5</v>
       </c>
       <c r="Q28" s="2">
-        <f t="shared" si="11"/>
-        <v>0.17676767676767677</v>
+        <f>P28/$P$31</f>
+        <v>0.37878787878787878</v>
       </c>
     </row>
     <row r="29" spans="11:20" x14ac:dyDescent="0.25">
       <c r="K29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L29" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M29" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N29" s="10">
+        <v>1</v>
+      </c>
+      <c r="O29" s="10">
+        <v>3</v>
+      </c>
+      <c r="P29" s="10">
+        <f t="shared" si="5"/>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="Q29" s="2">
+        <f>P29/$P$31</f>
+        <v>0.17676767676767677</v>
+      </c>
+    </row>
+    <row r="30" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L30" s="10">
         <v>0.2</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M30" s="10">
         <v>0.2</v>
       </c>
-      <c r="N29" s="10">
+      <c r="N30" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="O29" s="10">
-        <v>1</v>
-      </c>
-      <c r="P29" s="10">
-        <f t="shared" si="10"/>
+      <c r="O30" s="10">
+        <v>1</v>
+      </c>
+      <c r="P30" s="10">
+        <f t="shared" si="5"/>
         <v>0.43333333333333335</v>
       </c>
-      <c r="Q29" s="2">
-        <f t="shared" si="11"/>
+      <c r="Q30" s="2">
+        <f>P30/$P$31</f>
         <v>6.5656565656565663E-2</v>
       </c>
     </row>
-    <row r="30" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="10">
-        <f>SUM(P26:P29)</f>
+    <row r="31" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="10">
+        <f>SUM(P27:P30)</f>
         <v>6.6</v>
       </c>
-      <c r="Q30" s="2"/>
+      <c r="Q31" s="2"/>
     </row>
     <row r="33" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K33" s="2"/>
-      <c r="L33" s="2" t="s">
+      <c r="K33" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="L33" s="22"/>
+    </row>
+    <row r="34" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="M34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N33" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O33" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P33" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q33" s="2" t="s">
+      <c r="Q34" s="2" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L34" s="10">
-        <v>1</v>
-      </c>
-      <c r="M34" s="10">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="N34" s="10">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="O34" s="10">
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="P34" s="10">
-        <f>AVERAGE(L34:O34)</f>
-        <v>0.45238095238095233</v>
-      </c>
-      <c r="Q34" s="2">
-        <f>P34/$P$38</f>
-        <v>6.3844086021505375E-2</v>
       </c>
     </row>
     <row r="35" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K35" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L35" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M35" s="10">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N35" s="10">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O35" s="10">
-        <v>0.33333333333333331</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="P35" s="10">
-        <f t="shared" ref="P35:P37" si="12">AVERAGE(L35:O35)</f>
-        <v>1.3333333333333333</v>
+        <f>AVERAGE(L35:O35)</f>
+        <v>0.45238095238095233</v>
       </c>
       <c r="Q35" s="2">
-        <f t="shared" ref="Q35:Q37" si="13">P35/$P$38</f>
-        <v>0.18817204301075269</v>
+        <f>P35/$P$39</f>
+        <v>6.3844086021505375E-2</v>
       </c>
     </row>
     <row r="36" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L36" s="10">
         <v>3</v>
@@ -2005,103 +2095,109 @@
         <v>1</v>
       </c>
       <c r="O36" s="10">
-        <v>0.2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="P36" s="10">
-        <f t="shared" si="12"/>
-        <v>1.3</v>
+        <f t="shared" ref="P36:P38" si="6">AVERAGE(L36:O36)</f>
+        <v>1.3333333333333333</v>
       </c>
       <c r="Q36" s="2">
-        <f t="shared" si="13"/>
-        <v>0.18346774193548387</v>
+        <f>P36/$P$39</f>
+        <v>0.18817204301075269</v>
       </c>
     </row>
     <row r="37" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L37" s="10">
+        <v>3</v>
+      </c>
+      <c r="M37" s="10">
+        <v>1</v>
+      </c>
+      <c r="N37" s="10">
+        <v>1</v>
+      </c>
+      <c r="O37" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="P37" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="Q37" s="2">
+        <f>P37/$P$39</f>
+        <v>0.18346774193548387</v>
+      </c>
+    </row>
+    <row r="38" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L37" s="10">
+      <c r="L38" s="10">
         <v>7</v>
       </c>
-      <c r="M37" s="10">
+      <c r="M38" s="10">
         <v>3</v>
       </c>
-      <c r="N37" s="10">
+      <c r="N38" s="10">
         <v>5</v>
       </c>
-      <c r="O37" s="10">
-        <v>1</v>
-      </c>
-      <c r="P37" s="10">
-        <f t="shared" si="12"/>
+      <c r="O38" s="10">
+        <v>1</v>
+      </c>
+      <c r="P38" s="10">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="Q37" s="2">
-        <f t="shared" si="13"/>
+      <c r="Q38" s="2">
+        <f>P38/$P$39</f>
         <v>0.56451612903225812</v>
       </c>
     </row>
-    <row r="38" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="10">
-        <f>SUM(P34:P37)</f>
+    <row r="39" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="10">
+        <f>SUM(P35:P38)</f>
         <v>7.0857142857142854</v>
       </c>
-      <c r="Q38" s="2"/>
+      <c r="Q39" s="2"/>
     </row>
     <row r="41" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K41" s="2"/>
-      <c r="L41" s="2" t="s">
+      <c r="K41" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="L41" s="22"/>
+    </row>
+    <row r="42" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="M42" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N41" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="O42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P41" s="2" t="s">
+      <c r="P42" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="Q41" s="2" t="s">
+      <c r="Q42" s="2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L42" s="10">
-        <v>1</v>
-      </c>
-      <c r="M42" s="10">
-        <v>1</v>
-      </c>
-      <c r="N42" s="10">
-        <v>1</v>
-      </c>
-      <c r="O42" s="10">
-        <v>3</v>
-      </c>
-      <c r="P42" s="10">
-        <f>AVERAGE(L42:O42)</f>
-        <v>1.5</v>
-      </c>
-      <c r="Q42" s="2">
-        <f>P42/$P$46</f>
-        <v>0.3</v>
       </c>
     </row>
     <row r="43" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K43" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L43" s="10">
         <v>1</v>
@@ -2116,17 +2212,17 @@
         <v>3</v>
       </c>
       <c r="P43" s="10">
-        <f t="shared" ref="P43:P45" si="14">AVERAGE(L43:O43)</f>
+        <f>AVERAGE(L43:O43)</f>
         <v>1.5</v>
       </c>
       <c r="Q43" s="2">
-        <f t="shared" ref="Q43:Q45" si="15">P43/$P$46</f>
+        <f>P43/$P$47</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="44" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L44" s="10">
         <v>1</v>
@@ -2141,55 +2237,87 @@
         <v>3</v>
       </c>
       <c r="P44" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="P44:P46" si="7">AVERAGE(L44:O44)</f>
         <v>1.5</v>
       </c>
       <c r="Q44" s="2">
-        <f t="shared" si="15"/>
+        <f>P44/$P$47</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="45" spans="11:17" x14ac:dyDescent="0.25">
       <c r="K45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L45" s="10">
+        <v>1</v>
+      </c>
+      <c r="M45" s="10">
+        <v>1</v>
+      </c>
+      <c r="N45" s="10">
+        <v>1</v>
+      </c>
+      <c r="O45" s="10">
+        <v>3</v>
+      </c>
+      <c r="P45" s="10">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="Q45" s="2">
+        <f>P45/$P$47</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="46" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K46" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L45" s="10">
+      <c r="L46" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="M45" s="10">
+      <c r="M46" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="N45" s="10">
+      <c r="N46" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="O45" s="10">
-        <v>1</v>
-      </c>
-      <c r="P45" s="10">
-        <f t="shared" si="14"/>
+      <c r="O46" s="10">
+        <v>1</v>
+      </c>
+      <c r="P46" s="10">
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="Q45" s="2">
-        <f t="shared" si="15"/>
+      <c r="Q46" s="2">
+        <f>P46/$P$47</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="46" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="10">
-        <f>SUM(P42:P45)</f>
+    <row r="47" spans="11:17" x14ac:dyDescent="0.25">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="10">
+        <f>SUM(P43:P46)</f>
         <v>5</v>
       </c>
-      <c r="Q46" s="2"/>
+      <c r="Q47" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="S18:S19"/>
-    <mergeCell ref="T18:T19"/>
+  <mergeCells count="9">
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="T19:T20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="73" orientation="landscape" r:id="rId1"/>

</xml_diff>